<commit_message>
Added WebDriver  configuration for firefox,edge and safari
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\pup-platform-automation\pup-qa-pilot-automation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0146B1D1-298F-4144-A8B4-1186603C3061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF03B47-619F-47F0-A67F-971567F3D93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="90">
   <si>
     <t>Scenario_ID</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>STOP_PROCESSING</t>
+  </si>
+  <si>
+    <t>edge</t>
   </si>
 </sst>
 </file>
@@ -624,7 +627,7 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -669,7 +672,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>10</v>
@@ -689,7 +692,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>10</v>
@@ -729,7 +732,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>10</v>
@@ -1789,9 +1792,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1885,10 +1888,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>44</v>
@@ -1950,7 +1953,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>46</v>
@@ -2071,10 +2074,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>47</v>
@@ -2133,10 +2136,10 @@
         <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>45</v>
@@ -3001,10 +3004,10 @@
         <v>84</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
QAM-175 modified test data
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\pup-platform-automation\pup-qa-pilot-automation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF03B47-619F-47F0-A67F-971567F3D93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4E3C9D-276F-482B-AE63-A0B8D400721A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1794,7 +1794,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4042,6 +4042,11 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="please make a valid selection" promptTitle="browser selection" prompt="select the browser from the dropdown list" sqref="C2:C20" xr:uid="{170F0B8C-354D-49CD-900E-8B48951A9305}">
+      <formula1>"chrome,edge,firefox,safari"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>